<commit_message>
Amélioration modèle logique posologie - ajout d'exemples (#111)
* update poso examples

* update

* update

* Update posologie.fsh

* Update posologie.fsh

* Update posologie.fsh

* Update posologie.fsh

* Update posologie.fsh

* update poso

* update poso

* update poso descr

* update example

* update lignePrescription

* update quantitePrescrite 1f37966f1c321db3d92c5d8a4b8f95eea598151f
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-fr-current-medication-composition.xlsx
+++ b/main/ig/StructureDefinition-fr-current-medication-composition.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-21T08:04:49+00:00</t>
+    <t>2025-09-23T14:10:57+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -379,7 +379,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>
@@ -615,7 +615,7 @@
     <t>High-level kind of a clinical document at a macro level.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/document-classcodes</t>
+    <t>http://hl7.org/fhir/ValueSet/document-classcodes|4.0.1</t>
   </si>
   <si>
     <t>Event.subject</t>
@@ -731,7 +731,7 @@
     <t>Aa resource (or, for logical models, the URI of the logical model).</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/resource-types</t>
+    <t>http://hl7.org/fhir/ValueSet/resource-types|4.0.1</t>
   </si>
   <si>
     <t>Reference.type</t>
@@ -1034,7 +1034,7 @@
     <t>Composition.custodian</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization)
+    <t xml:space="preserve">Reference(Organization|4.0.1)
 </t>
   </si>
   <si>
@@ -1120,7 +1120,7 @@
   </si>
   <si>
     <t>Identifier
-Reference(Composition)</t>
+Reference(Composition|4.0.1)</t>
   </si>
   <si>
     <t>Target of the relationship</t>
@@ -1211,7 +1211,7 @@
     <t>Composition.event.detail</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Resource)
+    <t xml:space="preserve">Reference(Resource|4.0.1)
 </t>
   </si>
   <si>
@@ -1299,13 +1299,13 @@
     <t>Classification of a section of a composition/document.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/doc-section-codes</t>
+    <t>http://hl7.org/fhir/ValueSet/doc-section-codes|4.0.1</t>
   </si>
   <si>
     <t>Composition.section.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Device|Patient|RelatedPerson|Organization)
+    <t xml:space="preserve">Reference(Practitioner|4.0.1|PractitionerRole|4.0.1|Device|4.0.1|Patient|4.0.1|RelatedPerson|4.0.1|Organization|4.0.1)
 </t>
   </si>
   <si>
@@ -1401,7 +1401,7 @@
     <t>What order applies to the items in the entry.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/list-order</t>
+    <t>http://hl7.org/fhir/ValueSet/list-order|4.0.1</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode=COMP].sequenceNumber &gt; 1</t>
@@ -1454,7 +1454,7 @@
     <t>If a section is empty, why it is empty.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/list-empty-reason</t>
+    <t>http://hl7.org/fhir/ValueSet/list-empty-reason|4.0.1</t>
   </si>
   <si>
     <t>.inboundRelationship[typeCode=SUBJ,code&lt;ListEmptyReason].value[type=CD]</t>
@@ -1813,7 +1813,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="84.6171875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="93.98828125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>